<commit_message>
add original dynamic track rate
</commit_message>
<xml_diff>
--- a/aet_tool/control/sample_graph/aet_sample_result.xlsx
+++ b/aet_tool/control/sample_graph/aet_sample_result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -1839,7 +1839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -2152,7 +2152,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.25"/>
@@ -2287,26 +2287,26 @@
       <c r="B5" s="2">
         <v>586</v>
       </c>
-      <c r="C5" s="2">
-        <v>655</v>
+      <c r="C5" s="1">
+        <v>631</v>
       </c>
       <c r="D5" s="1">
-        <v>1950679412543</v>
+        <v>1950961273508</v>
       </c>
       <c r="E5" s="1">
-        <v>3116581</v>
+        <v>3157573</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="0"/>
-        <v>625903.646509749</v>
+        <f>D5/E5</f>
+        <v>617867.35366308235</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="1"/>
-        <v>1.1177474402730376</v>
+        <v>1.0767918088737201</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="2"/>
-        <v>4758.1389312977099</v>
+        <v>5004.07765451664</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2453,6 +2453,9 @@
         <f t="shared" si="2"/>
         <v>63.157303370786515</v>
       </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D13" s="2"/>
@@ -2470,7 +2473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>

</xml_diff>